<commit_message>
P06 Trial Run  ~ 3/6/23
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="185">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -569,6 +569,12 @@
   </si>
   <si>
     <t xml:space="preserve">Add git commit -m "P06 Trial Run 3/6/23” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write Listeners Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Cust to GitHub  ~ 3/6/23 12:36 PM"</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1060,7 +1066,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1212,11 +1218,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84063333"/>
-        <c:axId val="2959231"/>
+        <c:axId val="97559185"/>
+        <c:axId val="63983387"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84063333"/>
+        <c:axId val="97559185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1283,12 +1289,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2959231"/>
+        <c:crossAx val="63983387"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2959231"/>
+        <c:axId val="63983387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1363,7 +1369,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84063333"/>
+        <c:crossAx val="97559185"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1390,7 +1396,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1518,11 +1524,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="77776210"/>
-        <c:axId val="81930492"/>
+        <c:axId val="49761966"/>
+        <c:axId val="10526486"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77776210"/>
+        <c:axId val="49761966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,7 +1593,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81930492"/>
+        <c:crossAx val="10526486"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1595,7 +1601,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81930492"/>
+        <c:axId val="10526486"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1675,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77776210"/>
+        <c:crossAx val="49761966"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1696,7 +1702,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1788,28 +1794,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1824,11 +1830,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="58774670"/>
-        <c:axId val="61558042"/>
+        <c:axId val="90888843"/>
+        <c:axId val="82056035"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58774670"/>
+        <c:axId val="90888843"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1893,7 +1899,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61558042"/>
+        <c:crossAx val="82056035"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1901,7 +1907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61558042"/>
+        <c:axId val="82056035"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,7 +1981,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58774670"/>
+        <c:crossAx val="90888843"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2002,7 +2008,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2130,11 +2136,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="12058871"/>
-        <c:axId val="97922230"/>
+        <c:axId val="94920672"/>
+        <c:axId val="39896455"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="12058871"/>
+        <c:axId val="94920672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,7 +2205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97922230"/>
+        <c:crossAx val="39896455"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2207,7 +2213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97922230"/>
+        <c:axId val="39896455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2281,7 +2287,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12058871"/>
+        <c:crossAx val="94920672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2308,7 +2314,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2436,11 +2442,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49593997"/>
-        <c:axId val="78405610"/>
+        <c:axId val="31374676"/>
+        <c:axId val="97567194"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49593997"/>
+        <c:axId val="31374676"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2511,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78405610"/>
+        <c:crossAx val="97567194"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2513,7 +2519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78405610"/>
+        <c:axId val="97567194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2587,7 +2593,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49593997"/>
+        <c:crossAx val="31374676"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2614,7 +2620,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2742,11 +2748,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="84913053"/>
-        <c:axId val="39888468"/>
+        <c:axId val="31134479"/>
+        <c:axId val="73343364"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84913053"/>
+        <c:axId val="31134479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,7 +2817,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39888468"/>
+        <c:crossAx val="73343364"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2819,7 +2825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39888468"/>
+        <c:axId val="73343364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2893,7 +2899,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84913053"/>
+        <c:crossAx val="31134479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2920,7 +2926,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3048,11 +3054,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="91199906"/>
-        <c:axId val="30873951"/>
+        <c:axId val="22894863"/>
+        <c:axId val="24772493"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91199906"/>
+        <c:axId val="22894863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3117,7 +3123,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30873951"/>
+        <c:crossAx val="24772493"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3125,7 +3131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30873951"/>
+        <c:axId val="24772493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3205,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91199906"/>
+        <c:crossAx val="22894863"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3479,8 +3485,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6681,7 +6687,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6773,7 +6779,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -6786,7 +6792,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6802,7 +6808,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6818,7 +6824,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6834,7 +6840,7 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6850,7 +6856,7 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6866,7 +6872,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6882,7 +6888,7 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6964,24 +6970,36 @@
       </c>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="42"/>
+      <c r="B20" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="44"/>
+      <c r="D20" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>42</v>
+      </c>
       <c r="F20" s="45"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="42"/>
+      <c r="B21" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="44"/>
+      <c r="D21" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>42</v>
+      </c>
       <c r="F21" s="45"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11221,7 +11239,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>1</v>
@@ -11418,7 +11436,7 @@
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="48" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>

</xml_diff>

<commit_message>
P06 Trial Run  ~ 3/7/23
</commit_message>
<xml_diff>
--- a/P06/Scrum_Sprint_2.xlsx
+++ b/P06/Scrum_Sprint_2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="186">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add Cust to GitHub  ~ 3/6/23 12:36 PM"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add INSCO to GitHub  ~ 3/6/23"</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1066,7 +1069,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1218,11 +1221,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="97559185"/>
-        <c:axId val="63983387"/>
+        <c:axId val="6445248"/>
+        <c:axId val="33741303"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97559185"/>
+        <c:axId val="6445248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1289,12 +1292,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63983387"/>
+        <c:crossAx val="33741303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63983387"/>
+        <c:axId val="33741303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1369,7 +1372,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97559185"/>
+        <c:crossAx val="6445248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1396,7 +1399,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1524,11 +1527,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="49761966"/>
-        <c:axId val="10526486"/>
+        <c:axId val="6333024"/>
+        <c:axId val="3168857"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="49761966"/>
+        <c:axId val="6333024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,7 +1596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10526486"/>
+        <c:crossAx val="3168857"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1601,7 +1604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10526486"/>
+        <c:axId val="3168857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,7 +1678,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49761966"/>
+        <c:crossAx val="6333024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1702,7 +1705,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1794,28 +1797,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1830,11 +1833,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="90888843"/>
-        <c:axId val="82056035"/>
+        <c:axId val="82538374"/>
+        <c:axId val="71386839"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90888843"/>
+        <c:axId val="82538374"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1899,7 +1902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82056035"/>
+        <c:crossAx val="71386839"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1907,7 +1910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82056035"/>
+        <c:axId val="71386839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,7 +1984,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90888843"/>
+        <c:crossAx val="82538374"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2008,7 +2011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2136,11 +2139,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="94920672"/>
-        <c:axId val="39896455"/>
+        <c:axId val="20693522"/>
+        <c:axId val="89449618"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94920672"/>
+        <c:axId val="20693522"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2205,7 +2208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39896455"/>
+        <c:crossAx val="89449618"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2213,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39896455"/>
+        <c:axId val="89449618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2287,7 +2290,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94920672"/>
+        <c:crossAx val="20693522"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2314,7 +2317,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2442,11 +2445,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="31374676"/>
-        <c:axId val="97567194"/>
+        <c:axId val="84609684"/>
+        <c:axId val="40742105"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31374676"/>
+        <c:axId val="84609684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2514,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97567194"/>
+        <c:crossAx val="40742105"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2519,7 +2522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97567194"/>
+        <c:axId val="40742105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2593,7 +2596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31374676"/>
+        <c:crossAx val="84609684"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2620,7 +2623,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2748,11 +2751,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="31134479"/>
-        <c:axId val="73343364"/>
+        <c:axId val="5117511"/>
+        <c:axId val="76867293"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31134479"/>
+        <c:axId val="5117511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2817,7 +2820,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73343364"/>
+        <c:crossAx val="76867293"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2825,7 +2828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73343364"/>
+        <c:axId val="76867293"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +2902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31134479"/>
+        <c:crossAx val="5117511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2926,7 +2929,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3054,11 +3057,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="22894863"/>
-        <c:axId val="24772493"/>
+        <c:axId val="13855635"/>
+        <c:axId val="75242834"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22894863"/>
+        <c:axId val="13855635"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3123,7 +3126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24772493"/>
+        <c:crossAx val="75242834"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3131,7 +3134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24772493"/>
+        <c:axId val="75242834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3205,7 +3208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22894863"/>
+        <c:crossAx val="13855635"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3485,8 +3488,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4121,7 +4124,9 @@
       <c r="F31" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="G31" s="21"/>
+      <c r="G31" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="H31" s="22" t="s">
         <v>32</v>
       </c>
@@ -6687,7 +6692,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6779,7 +6784,7 @@
       </c>
       <c r="B7" s="32" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -6792,7 +6797,7 @@
       </c>
       <c r="B8" s="32" t="n">
         <f aca="false">B7-C8</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6808,7 +6813,7 @@
       </c>
       <c r="B9" s="32" t="n">
         <f aca="false">B8-C9</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6824,7 +6829,7 @@
       </c>
       <c r="B10" s="32" t="n">
         <f aca="false">B9-C10</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6840,7 +6845,7 @@
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">B10-C11</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6856,7 +6861,7 @@
       </c>
       <c r="B12" s="32" t="n">
         <f aca="false">B11-C12</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C12" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6872,7 +6877,7 @@
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">B12-C13</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6888,11 +6893,11 @@
       </c>
       <c r="B14" s="32" t="n">
         <f aca="false">B13-C14</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="32" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -7002,24 +7007,36 @@
       </c>
       <c r="F21" s="45"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="42"/>
+      <c r="B22" s="42" t="s">
+        <v>30</v>
+      </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="44"/>
+      <c r="D22" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>173</v>
+      </c>
       <c r="F22" s="45"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="42"/>
+      <c r="B23" s="42" t="s">
+        <v>61</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>42</v>
+      </c>
       <c r="F23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11239,7 +11256,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>1</v>
@@ -11436,7 +11453,7 @@
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="48" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>

</xml_diff>